<commit_message>
update raw ann and preds
</commit_message>
<xml_diff>
--- a/data annotation/raw annotations (with model predictions)/for validation - 1000 docs - ori - MIMIC-III-rad (free text removed, with predictions).xlsx
+++ b/data annotation/raw annotations (with model predictions)/for validation - 1000 docs - ori - MIMIC-III-rad (free text removed, with predictions).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/hdong3_ed_ac_uk/Documents/writing-UoE/rare disease detection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanong/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{7413F1A4-E423-49F3-A2C1-7906B2660D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CDE295F-4C28-0542-B0AA-97750435774B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E9F035-51BC-404C-A967-72D49E371CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2791,9 +2791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y43" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH76" sqref="AH76"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>